<commit_message>
adding data and updating runtime
</commit_message>
<xml_diff>
--- a/_data/metadata.xlsx
+++ b/_data/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abrett76/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abrett76/github/memories-for-the-future-findingaid/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B642722F-016E-D442-A65D-A293BA2B6F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F48075-5162-7347-84AC-AB122E5CD632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{36383585-15B8-FD4A-A1C8-6D5B4157C664}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{36383585-15B8-FD4A-A1C8-6D5B4157C664}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="264">
   <si>
     <t>Title</t>
   </si>
@@ -459,6 +459,375 @@
   </si>
   <si>
     <t>DOCIP</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>yanapaq</t>
+  </si>
+  <si>
+    <t>docip</t>
+  </si>
+  <si>
+    <t>cendoc</t>
+  </si>
+  <si>
+    <t>upnfii-recommendations-database</t>
+  </si>
+  <si>
+    <t>2025-unpfii-information-guide</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>deskaheh</t>
+  </si>
+  <si>
+    <t>archivaria</t>
+  </si>
+  <si>
+    <t>references-bibliography</t>
+  </si>
+  <si>
+    <t>leave-of-nations-uno-archive</t>
+  </si>
+  <si>
+    <t>cendoc-subject-search</t>
+  </si>
+  <si>
+    <t>spi-youth-internvention</t>
+  </si>
+  <si>
+    <t>cendoc-cl2</t>
+  </si>
+  <si>
+    <t>lyons</t>
+  </si>
+  <si>
+    <t>Indigenous Peoples speak out at UN Permanent Forum</t>
+  </si>
+  <si>
+    <t>MAC: Mines and Communities</t>
+  </si>
+  <si>
+    <t>Doctrine of Discovery Booklet</t>
+  </si>
+  <si>
+    <t>AILA</t>
+  </si>
+  <si>
+    <t>https://aila.li/booklet</t>
+  </si>
+  <si>
+    <t>Pagans in the Promised Land: a Primer on Religious Freedom</t>
+  </si>
+  <si>
+    <t>doctrine-of-discovery</t>
+  </si>
+  <si>
+    <t>Steven-Newcomb</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/pagans-in-the-promised-land-a-primer-on-religious-freedom/</t>
+  </si>
+  <si>
+    <t>An Open Letter on “Indian Residential Schools”</t>
+  </si>
+  <si>
+    <t>Betty Lyons</t>
+  </si>
+  <si>
+    <t>We Remember the Stolen Generations</t>
+  </si>
+  <si>
+    <t>Global Indigenous Peoples Caucus Statement  2025</t>
+  </si>
+  <si>
+    <t>Global Indigenous Peoples Caucus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://aila.ngo/global-indigenous-peoples-caucus-statement-2025/ </t>
+  </si>
+  <si>
+    <t>Global Indigenous Women’s Caucus 2024</t>
+  </si>
+  <si>
+    <t>Global Indigenous Women’s Caucus</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/global-indigenous-womens-caucus-2024/</t>
+  </si>
+  <si>
+    <t>Global Indigenous People’s Caucus 2024</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/global-indigenous-peoples-caucus-2024/</t>
+  </si>
+  <si>
+    <t>2017 Global Indigenous Women’s Caucus Statement (GIWC)</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/GIWC-2017-Statement-final-.pdf</t>
+  </si>
+  <si>
+    <t>Outcome from the Global Indigenous Peoples Caucus Statement for UNPFII22 (2023)</t>
+  </si>
+  <si>
+    <t>Global Indigenous Women’s Caucus Statement</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/global-indigenous-peoples-caucus-statement-for-unpfii22/</t>
+  </si>
+  <si>
+    <t>Statement from the Global Indigenous Women’s Caucus GIWC 2024</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/statement-from-the-global-indigenous-womens-caucus-giwc-2024/</t>
+  </si>
+  <si>
+    <t>2024 Global Indigenous Peoples Caucus Statement</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/2024-global-indigenous-peoples-caucus-statement/</t>
+  </si>
+  <si>
+    <t>2025 Global Indigenous Women’s Caucus Statement</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/2025-global-indigenous-womens-caucus-statement/</t>
+  </si>
+  <si>
+    <t>GIWC</t>
+  </si>
+  <si>
+    <t>GIPC</t>
+  </si>
+  <si>
+    <t>UNPFII Intervention training</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/UNPFII-Intervention-training.pdf</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/PDF-Comite-Global-de-Mujeres-Indigenas.pdf</t>
+  </si>
+  <si>
+    <t>Bibliography_UNPFII_2024_EN</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/Bibliography_UNPFII_2024_EN.pdf</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/Nordic-Sami-Youth-Statement-2023.pdf</t>
+  </si>
+  <si>
+    <t>Fact Sheet on the UNPFII</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/FACT-SHEET-ON-THE-PERMANENT-FORUM-ON-INDIGENOUS-ISSUE.pdf</t>
+  </si>
+  <si>
+    <t>Fact Sheet EMRIP</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/Fact-Sheet-EMRIP.pdf</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/Leaflet6-The-Permanent-Forum-on-Indigenous-Issues.pdf</t>
+  </si>
+  <si>
+    <t>References_UNPFII_2017</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/References_UNPFII_2017.pdf</t>
+  </si>
+  <si>
+    <t>References_UNPFII_2016_EN</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2024/04/References_UNPFII_2016_EN.pdf</t>
+  </si>
+  <si>
+    <t>Preliminary Report on Doctrine of Discovery</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/DOD5.pdf</t>
+  </si>
+  <si>
+    <t>UN Handbook 2023-24</t>
+  </si>
+  <si>
+    <t>https://www.un.org/sexualviolenceinconflict/wp-content/uploads/2023/09/auto-draft/UN-Handbook-2023-24.pdf</t>
+  </si>
+  <si>
+    <t>The Haudenosaunee Thanksgiving address to the natural world</t>
+  </si>
+  <si>
+    <t>Comite Global de Mujeres Indigenas ‚ Espanol</t>
+  </si>
+  <si>
+    <t>American Indian Law Alliance</t>
+  </si>
+  <si>
+    <t>Nordic Saami Youth Statement 2023</t>
+  </si>
+  <si>
+    <t>Leaflet on The Permanent Forum on Indigenous Issues</t>
+  </si>
+  <si>
+    <t>https://americanindian.si.edu/environment/pdf/01_02_thanksgiving_address.pdf</t>
+  </si>
+  <si>
+    <t>UNPFII</t>
+  </si>
+  <si>
+    <t>EMRIP</t>
+  </si>
+  <si>
+    <t>Nuclear Reactors are Not Green</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2019/03/NukeRedPaper3-25-19.pdf</t>
+  </si>
+  <si>
+    <t>https://doctrineofdiscovery.org/blog/continuacion-dominacion/</t>
+  </si>
+  <si>
+    <t>Continuing Christian Domination - April Online</t>
+  </si>
+  <si>
+    <t>https://www.aprilonline.org/continuing-christian-domination/</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/02/AILA-Betty-Lyons-Expert-Group-Meeting-Statement-Jan-23-2018.pdf</t>
+  </si>
+  <si>
+    <t>Joint Intervention The Haudenosaunee and the American Indian Law Alliance</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/02/EMRIP-Intervention-Final.pdf</t>
+  </si>
+  <si>
+    <t>AILA Intervention Mohawk Nation Border Issues - UNPFII 14th Session</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2015/07/14th_Session_Future_Work_Border_Crossing_AILA_Intervention_Final.pdf</t>
+  </si>
+  <si>
+    <t>Intervention by Haudenosaunee and AILA at EMRIP 6th Session 2013</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/03/EMRIP_Intervention_Final.pdf</t>
+  </si>
+  <si>
+    <t>Haudenosaunee intervention on Principles of Good Governance - UNPFII 13th Session</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/03/Haudenosaunee_Intervention_UNPFII_2014_Final_Oren_added_language.pdf</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/03/TI_final_UNPFII_2014.pdf</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/03/Perm_Observer_Final_5.22.2014.pdf</t>
+  </si>
+  <si>
+    <t>Paper on the Adoption of the Declaration on the Rights of Indigenous Peoples 2007</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2018/03/AmIndLawAlliance2007.pdf</t>
+  </si>
+  <si>
+    <t>U.S. Report to the UN Human Rights Commission on the Universal Periodic Review</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/U.S.-Report-to-the-UN-UPR.pdf</t>
+  </si>
+  <si>
+    <t>Tonya Gonnella Frichner Statement in Response to the US Report</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/2010.09.20_Tonya-Frichner-Stmt-Re-US-Report-for-UPR1.pdf</t>
+  </si>
+  <si>
+    <t>Announcement of US Support for Declaration on the Rights of Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/USA-Statement-Support-for-IPs.pdf</t>
+  </si>
+  <si>
+    <t>Statement by the Permanent Observer of the Holy See</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/Holy-See.pdf</t>
+  </si>
+  <si>
+    <t>Intervention on the Issue of Hydrofracking</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/Hydrofracking-Intervention.pdf</t>
+  </si>
+  <si>
+    <t>Intervention on USA-Canadian Border Issue</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/Intervention-on-USA.pdf</t>
+  </si>
+  <si>
+    <t>Press Release Ambassador Rice Statement on US Support for the Declaration on the Rights of Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/USUN-PRESS-RELEASE1.pdf</t>
+  </si>
+  <si>
+    <t>Oren Lyons Statement on the Iroquois Nationals Passport/Visa Controversy</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/Oren-Lyons-Statement.pdf</t>
+  </si>
+  <si>
+    <t>Robert Staffanson Talk at Oren Lyons Birthday Celebration</t>
+  </si>
+  <si>
+    <t>https://aila.ngo/wp-content/uploads/2010/09/Oren-Lyons-Testimonial-II-0-NYC-20101.pdf</t>
+  </si>
+  <si>
+    <t>redpaper</t>
+  </si>
+  <si>
+    <t>Continuación de la dominación de la Cristiandad: una respuesta a la declaración de repudio del Vaticano a la Doctrina del Descubrimiento - Español</t>
+  </si>
+  <si>
+    <t>Oral intervention presented by Betty Lyons (Onondaga Nation) in "Regional cases of autonomy in the territories of Indigenous Peoples" at the UN International Expert Group Meeting, 23-25 January 2018.</t>
+  </si>
+  <si>
+    <t>Joseph J. Heath</t>
+  </si>
+  <si>
+    <t>Haudenosaunee Confederacy</t>
+  </si>
+  <si>
+    <t>Joint intervention on Territorial Integrity - UNPFII 13th Session</t>
+  </si>
+  <si>
+    <t>Joint intervention calling for Indigenous Nations permanent observer status - UNPFII 13th Session</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Vatican</t>
+  </si>
+  <si>
+    <t>Robert Staffanson</t>
   </si>
 </sst>
 </file>
@@ -466,9 +835,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -485,6 +854,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -506,10 +897,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -517,12 +909,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -855,786 +1260,1568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB0C55-584B-9146-8DDC-410B67D642C2}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="26.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="48" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:8" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="3">
+      <c r="E6" s="5">
         <v>45768</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3">
+      <c r="E8" s="5">
         <v>28825</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="3">
+      <c r="E9" s="5">
         <v>42836</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:8" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="5"/>
+      <c r="F14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="3">
+      <c r="E18" s="5">
         <v>41774</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="3">
+      <c r="E21" s="5">
         <v>45959</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="3">
+      <c r="E22" s="5">
         <v>41024</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:8" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.15">
+      <c r="A23" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="5"/>
+      <c r="F23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A24" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="3">
+      <c r="E24" s="5">
         <v>41992</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
+    <row r="25" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="D25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="5">
+        <v>41041</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="3">
+      <c r="E26" s="5">
         <v>44743</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A27" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3">
+      <c r="D27" s="1"/>
+      <c r="E27" s="5">
         <v>42826</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="3">
+      <c r="E28" s="5">
         <v>39339</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="5"/>
+      <c r="F30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="5"/>
+      <c r="F31" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="5"/>
+      <c r="F32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="5"/>
+      <c r="F34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="5"/>
+      <c r="F35" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A36" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="5"/>
+      <c r="F37" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:8" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="9"/>
+      <c r="G41" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F41" t="s">
+      <c r="H41" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="4">
+      <c r="E42" s="9">
         <v>37196</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" s="7" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="43" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="G43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="10">
+        <v>44201</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="10">
+        <v>44410</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" s="9">
+        <v>44469</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A47" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="H47" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A48" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="9">
+        <v>45402</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E49" s="9">
+        <v>45041</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="H50" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="H51" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A52" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E52" s="9">
+        <v>42842</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A54" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" s="9">
+        <v>45399</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A55" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" s="9">
+        <v>45775</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="H57" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="H58" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="H59" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="H60" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="H61" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E62" s="9"/>
+      <c r="H62" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E63" s="9"/>
+      <c r="H63" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" s="9"/>
+      <c r="H64" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" s="9"/>
+      <c r="H65" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E66" s="9"/>
+      <c r="H66" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E67" s="9"/>
+      <c r="H67" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="H68" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E69" s="9"/>
+      <c r="H69" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="H70" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="H71" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="H72" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="H73" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E74" s="9"/>
+      <c r="H74" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="H75" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E76" s="9"/>
+      <c r="H76" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E77" s="9"/>
+      <c r="H77" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E78" s="9"/>
+      <c r="H78" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="H79" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E80" s="9"/>
+      <c r="H80" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="H81" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="H82" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E83" s="9"/>
+      <c r="H83" s="7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E84" s="9"/>
+      <c r="H84" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E85" s="9"/>
+      <c r="H85" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="H86" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E87" s="9"/>
+      <c r="H87" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E88" s="9"/>
+      <c r="H88" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H25" r:id="rId1" xr:uid="{A1AFF111-BBD6-234B-ABC6-BA31A2B4B083}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>